<commit_message>
almost finished p1 Unit 3.1
</commit_message>
<xml_diff>
--- a/Assignments deadline.xlsx
+++ b/Assignments deadline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Unit</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>D1</t>
+  </si>
+  <si>
+    <t>Just D2</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
   <dimension ref="B1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,10 +652,14 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42488</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">

</xml_diff>

<commit_message>
finished 17.3 me thinks
</commit_message>
<xml_diff>
--- a/Assignments deadline.xlsx
+++ b/Assignments deadline.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Unit</t>
   </si>
@@ -55,28 +55,31 @@
     <t>Unit 3</t>
   </si>
   <si>
+    <t>Not given</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Unit 5</t>
+  </si>
+  <si>
+    <t>P2,P3,M1</t>
+  </si>
+  <si>
+    <t>Unit 6</t>
+  </si>
+  <si>
+    <t>Soon as</t>
+  </si>
+  <si>
+    <t>Unit 17</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Unit 5</t>
-  </si>
-  <si>
-    <t>P2,P3,M1</t>
-  </si>
-  <si>
-    <t>Unit 6</t>
-  </si>
-  <si>
-    <t>Soon as</t>
-  </si>
-  <si>
-    <t>Unit 17</t>
-  </si>
-  <si>
-    <t>D1</t>
   </si>
   <si>
     <t>All of it, 2 criteria</t>
@@ -375,8 +378,8 @@
   </sheetPr>
   <dimension ref="B2:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -385,7 +388,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -492,7 +495,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -620,36 +623,25 @@
         <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E17" s="6" t="n">
         <v>42488</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="D3:D6,B3:F3">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+  <conditionalFormatting sqref="D7:D17">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"Resub"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D17">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>"Resub"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>